<commit_message>
Update CDE Ethnicity + CDE Katalog Logo
</commit_message>
<xml_diff>
--- a/output/ValueSet-vs-ethnic-groups.xlsx
+++ b/output/ValueSet-vs-ethnic-groups.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include from SNOMED CT" r:id="rId4" sheetId="2"/>
+    <sheet name="Exclude from SNOMED CT" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +58,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-05T02:26:26+01:00</t>
+    <t>2023-03-05T17:53:57+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -115,6 +116,12 @@
   </si>
   <si>
     <t>http://snomed.info/sct</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Ethnic group (ethnic group)</t>
   </si>
 </sst>
 </file>
@@ -430,4 +437,53 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="30.703125" customWidth="true"/>
+    <col min="2" max="2" width="50.703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>